<commit_message>
Updated equality codebook, and conducted regressions
</commit_message>
<xml_diff>
--- a/Data/EqualityCodebook.xlsx
+++ b/Data/EqualityCodebook.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bjr/GitHub/TransResearch2016/Data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24426"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="12040" yWindow="0" windowWidth="16740" windowHeight="11180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" refMode="R1C1" concurrentCalc="0"/>
+  <calcPr calcId="140001" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
   <si>
     <t>State</t>
   </si>
@@ -387,16 +382,111 @@
   </si>
   <si>
     <t>Transgender Exclusions in State Medicaid</t>
+  </si>
+  <si>
+    <t>superdomaDiff</t>
+  </si>
+  <si>
+    <t>domaDiff</t>
+  </si>
+  <si>
+    <t>trans_disDiff</t>
+  </si>
+  <si>
+    <t>gay_discDiff</t>
+  </si>
+  <si>
+    <t>Diffusion variable among the states for superDoma, unlagged</t>
+  </si>
+  <si>
+    <t>Diffusion variable among the states for doma unlagged</t>
+  </si>
+  <si>
+    <t>Diffusion variable among the states for transgender antidiscrimination statute (from trans_dis), unlagged</t>
+  </si>
+  <si>
+    <t>Diffusion variable among the states for gay antidiscrimination statute (from gay_disc), unlagged</t>
+  </si>
+  <si>
+    <t>lagged version of timeVar by one year</t>
+  </si>
+  <si>
+    <t>lagged version of timeVarDt by one year</t>
+  </si>
+  <si>
+    <t>the time varying columns in "ssph over time with williams.xlsx" converted to long format and merged with the rest of the data</t>
+  </si>
+  <si>
+    <t>lagged version of timeVarDtWl by one year</t>
+  </si>
+  <si>
+    <t>lagged version of timeVarWill by one year</t>
+  </si>
+  <si>
+    <t>the time varying columns in "ssphh over time with williams  straight line 1990 2008.xlsx", converted to long format and merged</t>
+  </si>
+  <si>
+    <t>the time varying computed williams measures in  "ssphh over time with williams  straight line 1990 2008.xlsx", converted to long format and merged</t>
+  </si>
+  <si>
+    <t>time varying computed williams measures in "ssphh over time with williams.xlsx" converted to long format and merged</t>
+  </si>
+  <si>
+    <t>timeVarWillLag</t>
+  </si>
+  <si>
+    <t>timeVarLag</t>
+  </si>
+  <si>
+    <t>timeVarDt</t>
+  </si>
+  <si>
+    <t>timeVarDtLag</t>
+  </si>
+  <si>
+    <t>timeVarDtWill</t>
+  </si>
+  <si>
+    <t>timeVarDtWillLag</t>
+  </si>
+  <si>
+    <t>timeVarWill</t>
+  </si>
+  <si>
+    <t>timeVar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -419,13 +509,41 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="13">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -481,7 +599,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -516,7 +634,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -693,7 +811,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -701,15 +819,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>89</v>
       </c>
@@ -717,7 +838,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -725,7 +846,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -733,7 +854,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -741,7 +862,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -749,7 +870,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -757,7 +878,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -765,7 +886,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -773,7 +894,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -781,7 +902,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -789,7 +910,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -797,7 +918,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -805,7 +926,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -813,7 +934,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -821,7 +942,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -829,7 +950,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -837,7 +958,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -845,7 +966,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -853,7 +974,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -861,7 +982,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -869,7 +990,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -877,7 +998,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -885,7 +1006,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -893,7 +1014,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -901,7 +1022,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -909,7 +1030,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -917,7 +1038,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -925,7 +1046,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -933,7 +1054,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -941,7 +1062,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -949,7 +1070,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -957,7 +1078,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -965,7 +1086,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -973,7 +1094,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -981,7 +1102,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -989,7 +1110,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -997,7 +1118,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1005,7 +1126,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1013,7 +1134,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1021,7 +1142,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1029,7 +1150,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1037,7 +1158,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1045,7 +1166,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1053,7 +1174,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1061,7 +1182,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1069,7 +1190,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1077,7 +1198,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -1085,7 +1206,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1093,7 +1214,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -1101,7 +1222,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -1109,7 +1230,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -1117,7 +1238,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -1125,7 +1246,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -1133,7 +1254,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -1141,7 +1262,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -1149,7 +1270,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -1157,7 +1278,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -1165,7 +1286,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -1173,7 +1294,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -1181,7 +1302,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -1189,7 +1310,109 @@
         <v>119</v>
       </c>
     </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>121</v>
+      </c>
+      <c r="B62" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>122</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>123</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B65" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B66" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B67" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B68" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B69" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B70" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B71" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B72" t="s">
+        <v>132</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>